<commit_message>
Piryankova mit viel Literatur hinzugefügt
</commit_message>
<xml_diff>
--- a/OverviewLiterature.xlsx
+++ b/OverviewLiterature.xlsx
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Jahr</t>
   </si>
   <si>
-    <t>Kürzel</t>
-  </si>
-  <si>
     <t>Entfernungen</t>
   </si>
   <si>
@@ -66,6 +63,48 @@
   </si>
   <si>
     <t>Teilnehmeranzahl</t>
+  </si>
+  <si>
+    <t>Piryankova</t>
+  </si>
+  <si>
+    <t>Erstautor</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>2-6m</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>1,5-6m</t>
+  </si>
+  <si>
+    <t>Trials</t>
+  </si>
+  <si>
+    <t>27-30</t>
+  </si>
+  <si>
+    <t>flat LSID</t>
+  </si>
+  <si>
+    <t>semi-spherical LSID</t>
+  </si>
+  <si>
+    <t>MPI cabin</t>
+  </si>
+  <si>
+    <t>2-5,5m</t>
+  </si>
+  <si>
+    <t>1,5-5,5m</t>
   </si>
 </sst>
 </file>
@@ -429,56 +468,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2013</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2">
+        <v>77</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="2" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5">
         <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>